<commit_message>
update leave card 02/13/2024 4;39pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA ACCOUNTING/ROMILLA, MARIBEL.xlsx
+++ b/CASUAL/LA ACCOUNTING/ROMILLA, MARIBEL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="139">
   <si>
     <t>PERIOD</t>
   </si>
@@ -448,6 +448,12 @@
   </si>
   <si>
     <t>UT(0-3-12)</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>FILIAL 01/24/2024</t>
   </si>
 </sst>
 </file>
@@ -829,20 +835,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -853,6 +859,9 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -862,14 +871,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1112,16 +1138,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1362,16 +1378,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1405,7 +1411,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1448,7 +1454,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1512,7 +1518,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1572,7 +1578,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1644,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1707,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1805,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1858,7 +1864,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1929,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1966,7 +1972,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2041,7 +2047,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2227,7 +2233,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2293,7 +2299,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2351,7 +2357,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2417,7 +2423,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2473,7 +2479,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2548,7 +2554,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2591,7 +2597,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2657,7 +2663,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2713,7 +2719,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2809,25 +2815,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K125" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K126" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="26"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="25"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="24"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="23"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="22">
+    <tableColumn id="1" name="PERIOD" dataDxfId="27"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="26"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="25"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="24"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="23">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="21"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="20">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="22"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="21">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="19"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="18">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="20"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="19">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="17"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="16"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="18"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2839,25 +2845,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K130" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="12"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="11"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="10"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="9"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="8">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="7"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="5"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="4">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="3"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3186,12 +3192,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K125"/>
+  <dimension ref="A2:K126"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3690" topLeftCell="A84" activePane="bottomLeft"/>
       <selection activeCell="E9" sqref="E9"/>
-      <selection pane="bottomLeft" activeCell="K96" sqref="K96"/>
+      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3213,38 +3219,38 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="54"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="55">
         <v>39085</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
@@ -3256,23 +3262,23 @@
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3298,18 +3304,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3356,7 +3362,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>56.017000000000003</v>
+        <v>59.767000000000003</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3366,7 +3372,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>39.5</v>
+        <v>43.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -5294,13 +5300,15 @@
         <v>45231</v>
       </c>
       <c r="B98" s="20"/>
-      <c r="C98" s="13"/>
+      <c r="C98" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D98" s="39"/>
       <c r="E98" s="9"/>
       <c r="F98" s="20"/>
-      <c r="G98" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G98" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H98" s="39"/>
       <c r="I98" s="9"/>
@@ -5312,13 +5320,15 @@
         <v>45261</v>
       </c>
       <c r="B99" s="20"/>
-      <c r="C99" s="13"/>
+      <c r="C99" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D99" s="39"/>
       <c r="E99" s="9"/>
       <c r="F99" s="20"/>
-      <c r="G99" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G99" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H99" s="39"/>
       <c r="I99" s="9"/>
@@ -5326,18 +5336,15 @@
       <c r="K99" s="20"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A100" s="40">
-        <v>45292</v>
+      <c r="A100" s="48" t="s">
+        <v>137</v>
       </c>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
       <c r="D100" s="39"/>
       <c r="E100" s="9"/>
       <c r="F100" s="20"/>
-      <c r="G100" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
+      <c r="G100" s="13"/>
       <c r="H100" s="39"/>
       <c r="I100" s="9"/>
       <c r="J100" s="11"/>
@@ -5345,25 +5352,31 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40">
-        <v>45323</v>
-      </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="13"/>
+        <v>45292</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D101" s="39"/>
       <c r="E101" s="9"/>
       <c r="F101" s="20"/>
-      <c r="G101" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G101" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H101" s="39"/>
       <c r="I101" s="9"/>
       <c r="J101" s="11"/>
-      <c r="K101" s="20"/>
+      <c r="K101" s="20" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40">
-        <v>45352</v>
+        <v>45323</v>
       </c>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -5381,7 +5394,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40">
-        <v>45383</v>
+        <v>45352</v>
       </c>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -5399,7 +5412,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -5417,7 +5430,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40">
-        <v>45444</v>
+        <v>45413</v>
       </c>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -5435,7 +5448,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40">
-        <v>45474</v>
+        <v>45444</v>
       </c>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -5453,7 +5466,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40">
-        <v>45505</v>
+        <v>45474</v>
       </c>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -5471,7 +5484,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40">
-        <v>45536</v>
+        <v>45505</v>
       </c>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -5489,7 +5502,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40">
-        <v>45566</v>
+        <v>45536</v>
       </c>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -5507,7 +5520,7 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40">
-        <v>45597</v>
+        <v>45566</v>
       </c>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -5525,7 +5538,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40">
-        <v>45627</v>
+        <v>45597</v>
       </c>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -5543,7 +5556,7 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40">
-        <v>45658</v>
+        <v>45627</v>
       </c>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -5561,7 +5574,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40">
-        <v>45689</v>
+        <v>45658</v>
       </c>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -5579,7 +5592,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40">
-        <v>45717</v>
+        <v>45689</v>
       </c>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5597,7 +5610,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40">
-        <v>45748</v>
+        <v>45717</v>
       </c>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5615,7 +5628,7 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40">
-        <v>45778</v>
+        <v>45748</v>
       </c>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5633,7 +5646,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40">
-        <v>45809</v>
+        <v>45778</v>
       </c>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5651,7 +5664,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40">
-        <v>45839</v>
+        <v>45809</v>
       </c>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5669,7 +5682,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40">
-        <v>45870</v>
+        <v>45839</v>
       </c>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5687,7 +5700,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40">
-        <v>45901</v>
+        <v>45870</v>
       </c>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5705,7 +5718,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40">
-        <v>45931</v>
+        <v>45901</v>
       </c>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5723,7 +5736,7 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40">
-        <v>45962</v>
+        <v>45931</v>
       </c>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5741,7 +5754,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40">
-        <v>45992</v>
+        <v>45962</v>
       </c>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5759,7 +5772,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40">
-        <v>46023</v>
+        <v>45992</v>
       </c>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5776,37 +5789,55 @@
       <c r="K124" s="20"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A125" s="41"/>
-      <c r="B125" s="15"/>
-      <c r="C125" s="42"/>
-      <c r="D125" s="43"/>
+      <c r="A125" s="40">
+        <v>46023</v>
+      </c>
+      <c r="B125" s="20"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="39"/>
       <c r="E125" s="9"/>
-      <c r="F125" s="15"/>
-      <c r="G125" s="42" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
-      </c>
-      <c r="H125" s="43"/>
+      <c r="F125" s="20"/>
+      <c r="G125" s="13" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H125" s="39"/>
       <c r="I125" s="9"/>
-      <c r="J125" s="12"/>
-      <c r="K125" s="15"/>
+      <c r="J125" s="11"/>
+      <c r="K125" s="20"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="41"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="42"/>
+      <c r="D126" s="43"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="42" t="str">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v/>
+      </c>
+      <c r="H126" s="43"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="12"/>
+      <c r="K126" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="K88:K89">
-    <cfRule type="timePeriod" dxfId="31" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(K88,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K88,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5843,10 +5874,10 @@
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A91" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3690" topLeftCell="A22" activePane="bottomLeft"/>
       <selection activeCell="D9" sqref="D9"/>
-      <selection pane="bottomLeft" activeCell="H105" sqref="H105"/>
+      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5868,38 +5899,38 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="54"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="55">
         <v>39085</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="53"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
@@ -5911,23 +5942,23 @@
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="50"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="54"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -5953,18 +5984,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -8154,7 +8185,7 @@
       <c r="H105" s="39"/>
       <c r="I105" s="9"/>
       <c r="J105" s="11"/>
-      <c r="K105" s="61">
+      <c r="K105" s="50">
         <v>45275</v>
       </c>
     </row>
@@ -8573,7 +8604,7 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <conditionalFormatting sqref="K98:K100">
-    <cfRule type="timePeriod" dxfId="15" priority="1" timePeriod="lastWeek">
+    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(K98,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(K98,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8626,17 +8657,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="J1" s="59" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="J1" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -8721,12 +8752,12 @@
         <v>30</v>
       </c>
       <c r="G6" s="46"/>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="37">

</xml_diff>